<commit_message>
Updated workflows, index.html, and other files
</commit_message>
<xml_diff>
--- a/locations/A15.xlsx
+++ b/locations/A15.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://comlineukcom-my.sharepoint.com/personal/jaydip_d_comline_uk_com/Documents/CAPLOCATION/Deployment/bulk_report_webapp/locations/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://comlineukcom-my.sharepoint.com/personal/jaydip_d_comline_uk_com/Documents/CAPLOCATION/Deployment/MYPROJECT-WORKING/locations/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="8_{C7431AD7-7F57-4367-B18E-E7DF7BC06822}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9136FCAA-8025-4F66-837A-BEAB6674995F}"/>
+  <xr:revisionPtr revIDLastSave="45" documentId="8_{C7431AD7-7F57-4367-B18E-E7DF7BC06822}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A6E82C4A-01FA-4364-9E83-FDD0A0B294AD}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="438" uniqueCount="396">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="461" uniqueCount="424">
   <si>
     <t>Bay:</t>
   </si>
@@ -1226,6 +1226,90 @@
   </si>
   <si>
     <t>05302G</t>
+  </si>
+  <si>
+    <t>09322A</t>
+  </si>
+  <si>
+    <t>09322B</t>
+  </si>
+  <si>
+    <t>09322C</t>
+  </si>
+  <si>
+    <t>09322D</t>
+  </si>
+  <si>
+    <t>09322E</t>
+  </si>
+  <si>
+    <t>09322F</t>
+  </si>
+  <si>
+    <t>09322G</t>
+  </si>
+  <si>
+    <t>09332A</t>
+  </si>
+  <si>
+    <t>09332B</t>
+  </si>
+  <si>
+    <t>09332C</t>
+  </si>
+  <si>
+    <t>09332D</t>
+  </si>
+  <si>
+    <t>09332E</t>
+  </si>
+  <si>
+    <t>09332F</t>
+  </si>
+  <si>
+    <t>09332G</t>
+  </si>
+  <si>
+    <t>09341A</t>
+  </si>
+  <si>
+    <t>09341B</t>
+  </si>
+  <si>
+    <t>09341C</t>
+  </si>
+  <si>
+    <t>09341D</t>
+  </si>
+  <si>
+    <t>09341E</t>
+  </si>
+  <si>
+    <t>09341F</t>
+  </si>
+  <si>
+    <t>09341G</t>
+  </si>
+  <si>
+    <t>09342A</t>
+  </si>
+  <si>
+    <t>09342B</t>
+  </si>
+  <si>
+    <t>09342C</t>
+  </si>
+  <si>
+    <t>09342D</t>
+  </si>
+  <si>
+    <t>09342E</t>
+  </si>
+  <si>
+    <t>09342F</t>
+  </si>
+  <si>
+    <t>09342G</t>
   </si>
 </sst>
 </file>
@@ -1282,7 +1366,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -1370,11 +1454,57 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1441,14 +1571,30 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1783,83 +1929,87 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AD32"/>
+  <dimension ref="A1:AF32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AH18" sqref="AH18"/>
+      <selection pane="topRight" activeCell="AF22" sqref="AF22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="2" width="7" customWidth="1"/>
-    <col min="3" max="30" width="22.81640625" style="1" customWidth="1"/>
+    <col min="3" max="32" width="22.81640625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="4"/>
-      <c r="C1" s="23">
+      <c r="C1" s="26">
         <v>1</v>
       </c>
-      <c r="D1" s="24"/>
-      <c r="E1" s="23">
+      <c r="D1" s="27"/>
+      <c r="E1" s="26">
         <v>2</v>
       </c>
-      <c r="F1" s="24"/>
-      <c r="G1" s="23">
+      <c r="F1" s="27"/>
+      <c r="G1" s="26">
         <v>3</v>
       </c>
-      <c r="H1" s="24"/>
-      <c r="I1" s="23">
+      <c r="H1" s="27"/>
+      <c r="I1" s="26">
         <v>4</v>
       </c>
-      <c r="J1" s="24"/>
-      <c r="K1" s="23">
+      <c r="J1" s="27"/>
+      <c r="K1" s="26">
         <v>5</v>
       </c>
-      <c r="L1" s="24"/>
-      <c r="M1" s="23">
+      <c r="L1" s="27"/>
+      <c r="M1" s="26">
         <v>6</v>
       </c>
-      <c r="N1" s="24"/>
-      <c r="O1" s="23">
+      <c r="N1" s="27"/>
+      <c r="O1" s="26">
         <v>7</v>
       </c>
-      <c r="P1" s="24"/>
-      <c r="Q1" s="23">
+      <c r="P1" s="27"/>
+      <c r="Q1" s="26">
         <v>8</v>
       </c>
-      <c r="R1" s="24"/>
-      <c r="S1" s="23">
+      <c r="R1" s="27"/>
+      <c r="S1" s="26">
         <v>9</v>
       </c>
-      <c r="T1" s="24"/>
-      <c r="U1" s="23">
+      <c r="T1" s="27"/>
+      <c r="U1" s="26">
         <v>10</v>
       </c>
-      <c r="V1" s="24"/>
-      <c r="W1" s="23">
+      <c r="V1" s="27"/>
+      <c r="W1" s="26">
         <v>11</v>
       </c>
-      <c r="X1" s="24"/>
-      <c r="Y1" s="23">
+      <c r="X1" s="27"/>
+      <c r="Y1" s="26">
         <v>12</v>
       </c>
-      <c r="Z1" s="24"/>
-      <c r="AA1" s="23">
+      <c r="Z1" s="27"/>
+      <c r="AA1" s="26">
         <v>13</v>
       </c>
-      <c r="AB1" s="24"/>
-      <c r="AC1" s="23">
+      <c r="AB1" s="27"/>
+      <c r="AC1" s="26">
         <v>14</v>
       </c>
-      <c r="AD1" s="24"/>
+      <c r="AD1" s="27"/>
+      <c r="AE1" s="26">
+        <v>15</v>
+      </c>
+      <c r="AF1" s="27"/>
     </row>
-    <row r="2" spans="1:30" x14ac:dyDescent="0.35">
-      <c r="A2" s="25" t="s">
+    <row r="2" spans="1:32" x14ac:dyDescent="0.35">
+      <c r="A2" s="23" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
@@ -1949,9 +2099,13 @@
       <c r="AD2" s="15" t="s">
         <v>389</v>
       </c>
+      <c r="AE2" s="15" t="s">
+        <v>395</v>
+      </c>
+      <c r="AF2" s="15"/>
     </row>
-    <row r="3" spans="1:30" x14ac:dyDescent="0.35">
-      <c r="A3" s="26"/>
+    <row r="3" spans="1:32" x14ac:dyDescent="0.35">
+      <c r="A3" s="24"/>
       <c r="B3" s="7"/>
       <c r="C3" s="21"/>
       <c r="D3" s="19"/>
@@ -1981,9 +2135,11 @@
       <c r="AB3" s="4"/>
       <c r="AC3" s="4"/>
       <c r="AD3" s="20"/>
+      <c r="AE3" s="20"/>
+      <c r="AF3" s="20"/>
     </row>
-    <row r="4" spans="1:30" x14ac:dyDescent="0.35">
-      <c r="A4" s="26"/>
+    <row r="4" spans="1:32" x14ac:dyDescent="0.35">
+      <c r="A4" s="24"/>
       <c r="B4" s="7" t="s">
         <v>30</v>
       </c>
@@ -2071,9 +2227,13 @@
       <c r="AD4" s="15" t="s">
         <v>388</v>
       </c>
+      <c r="AE4" s="15" t="s">
+        <v>394</v>
+      </c>
+      <c r="AF4" s="15"/>
     </row>
-    <row r="5" spans="1:30" x14ac:dyDescent="0.35">
-      <c r="A5" s="26"/>
+    <row r="5" spans="1:32" x14ac:dyDescent="0.35">
+      <c r="A5" s="24"/>
       <c r="B5" s="7"/>
       <c r="C5" s="21"/>
       <c r="D5" s="19"/>
@@ -2103,9 +2263,11 @@
       <c r="AB5" s="4"/>
       <c r="AC5" s="4"/>
       <c r="AD5" s="20"/>
+      <c r="AE5" s="20"/>
+      <c r="AF5" s="20"/>
     </row>
-    <row r="6" spans="1:30" x14ac:dyDescent="0.35">
-      <c r="A6" s="26"/>
+    <row r="6" spans="1:32" x14ac:dyDescent="0.35">
+      <c r="A6" s="24"/>
       <c r="B6" s="7" t="s">
         <v>58</v>
       </c>
@@ -2193,9 +2355,13 @@
       <c r="AD6" s="15" t="s">
         <v>387</v>
       </c>
+      <c r="AE6" s="15" t="s">
+        <v>393</v>
+      </c>
+      <c r="AF6" s="15"/>
     </row>
-    <row r="7" spans="1:30" x14ac:dyDescent="0.35">
-      <c r="A7" s="26"/>
+    <row r="7" spans="1:32" x14ac:dyDescent="0.35">
+      <c r="A7" s="24"/>
       <c r="B7" s="7"/>
       <c r="C7" s="21"/>
       <c r="D7" s="19"/>
@@ -2225,9 +2391,11 @@
       <c r="AB7" s="4"/>
       <c r="AC7" s="4"/>
       <c r="AD7" s="20"/>
+      <c r="AE7" s="20"/>
+      <c r="AF7" s="20"/>
     </row>
-    <row r="8" spans="1:30" x14ac:dyDescent="0.35">
-      <c r="A8" s="26"/>
+    <row r="8" spans="1:32" x14ac:dyDescent="0.35">
+      <c r="A8" s="24"/>
       <c r="B8" s="7" t="s">
         <v>86</v>
       </c>
@@ -2315,9 +2483,13 @@
       <c r="AD8" s="15" t="s">
         <v>386</v>
       </c>
+      <c r="AE8" s="15" t="s">
+        <v>392</v>
+      </c>
+      <c r="AF8" s="15"/>
     </row>
-    <row r="9" spans="1:30" x14ac:dyDescent="0.35">
-      <c r="A9" s="26"/>
+    <row r="9" spans="1:32" x14ac:dyDescent="0.35">
+      <c r="A9" s="24"/>
       <c r="B9" s="7"/>
       <c r="C9" s="21"/>
       <c r="D9" s="19"/>
@@ -2347,9 +2519,11 @@
       <c r="AB9" s="4"/>
       <c r="AC9" s="4"/>
       <c r="AD9" s="20"/>
+      <c r="AE9" s="20"/>
+      <c r="AF9" s="20"/>
     </row>
-    <row r="10" spans="1:30" x14ac:dyDescent="0.35">
-      <c r="A10" s="26"/>
+    <row r="10" spans="1:32" x14ac:dyDescent="0.35">
+      <c r="A10" s="24"/>
       <c r="B10" s="7" t="s">
         <v>114</v>
       </c>
@@ -2437,9 +2611,13 @@
       <c r="AD10" s="15" t="s">
         <v>385</v>
       </c>
+      <c r="AE10" s="15" t="s">
+        <v>391</v>
+      </c>
+      <c r="AF10" s="15"/>
     </row>
-    <row r="11" spans="1:30" x14ac:dyDescent="0.35">
-      <c r="A11" s="26"/>
+    <row r="11" spans="1:32" x14ac:dyDescent="0.35">
+      <c r="A11" s="24"/>
       <c r="B11" s="7"/>
       <c r="C11" s="21"/>
       <c r="D11" s="19"/>
@@ -2469,9 +2647,11 @@
       <c r="AB11" s="4"/>
       <c r="AC11" s="4"/>
       <c r="AD11" s="20"/>
+      <c r="AE11" s="20"/>
+      <c r="AF11" s="20"/>
     </row>
-    <row r="12" spans="1:30" x14ac:dyDescent="0.35">
-      <c r="A12" s="26"/>
+    <row r="12" spans="1:32" x14ac:dyDescent="0.35">
+      <c r="A12" s="24"/>
       <c r="B12" s="7" t="s">
         <v>142</v>
       </c>
@@ -2559,9 +2739,13 @@
       <c r="AD12" s="15" t="s">
         <v>384</v>
       </c>
+      <c r="AE12" s="15" t="s">
+        <v>390</v>
+      </c>
+      <c r="AF12" s="15"/>
     </row>
-    <row r="13" spans="1:30" x14ac:dyDescent="0.35">
-      <c r="A13" s="26"/>
+    <row r="13" spans="1:32" x14ac:dyDescent="0.35">
+      <c r="A13" s="24"/>
       <c r="B13" s="7"/>
       <c r="C13" s="21"/>
       <c r="D13" s="4"/>
@@ -2591,9 +2775,11 @@
       <c r="AB13" s="4"/>
       <c r="AC13" s="4"/>
       <c r="AD13" s="20"/>
+      <c r="AE13" s="20"/>
+      <c r="AF13" s="20"/>
     </row>
-    <row r="14" spans="1:30" s="14" customFormat="1" ht="11" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="26"/>
+    <row r="14" spans="1:32" s="14" customFormat="1" ht="11" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="24"/>
       <c r="B14" s="13" t="s">
         <v>170</v>
       </c>
@@ -2681,9 +2867,13 @@
       <c r="AD14" s="15" t="s">
         <v>198</v>
       </c>
+      <c r="AE14" s="15" t="s">
+        <v>199</v>
+      </c>
+      <c r="AF14" s="15"/>
     </row>
-    <row r="15" spans="1:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="27"/>
+    <row r="15" spans="1:32" ht="16.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="25"/>
       <c r="B15" s="6"/>
       <c r="C15" s="21"/>
       <c r="D15" s="21"/>
@@ -2713,8 +2903,10 @@
       <c r="AB15" s="22"/>
       <c r="AC15" s="22"/>
       <c r="AD15" s="22"/>
+      <c r="AE15" s="17"/>
+      <c r="AF15" s="22"/>
     </row>
-    <row r="16" spans="1:30" ht="17" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:32" ht="17" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="3"/>
       <c r="B16" s="3"/>
       <c r="C16" s="3" t="s">
@@ -2801,165 +2993,181 @@
       <c r="AD16" s="3" t="s">
         <v>200</v>
       </c>
+      <c r="AE16" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="AF16" s="3" t="s">
+        <v>200</v>
+      </c>
     </row>
-    <row r="17" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A17" s="4" t="s">
         <v>0</v>
       </c>
       <c r="B17" s="4"/>
-      <c r="C17" s="23">
+      <c r="C17" s="26">
         <v>16</v>
       </c>
-      <c r="D17" s="24"/>
-      <c r="E17" s="23">
+      <c r="D17" s="27"/>
+      <c r="E17" s="26">
         <v>17</v>
       </c>
-      <c r="F17" s="24"/>
-      <c r="G17" s="23">
+      <c r="F17" s="27"/>
+      <c r="G17" s="26">
         <v>18</v>
       </c>
-      <c r="H17" s="24"/>
-      <c r="I17" s="23">
+      <c r="H17" s="27"/>
+      <c r="I17" s="26">
         <v>19</v>
       </c>
-      <c r="J17" s="24"/>
-      <c r="K17" s="23">
+      <c r="J17" s="27"/>
+      <c r="K17" s="26">
         <v>20</v>
       </c>
-      <c r="L17" s="24"/>
-      <c r="M17" s="23">
+      <c r="L17" s="27"/>
+      <c r="M17" s="26">
         <v>21</v>
       </c>
-      <c r="N17" s="24"/>
-      <c r="O17" s="23">
+      <c r="N17" s="27"/>
+      <c r="O17" s="26">
         <v>22</v>
       </c>
-      <c r="P17" s="24"/>
-      <c r="Q17" s="23">
+      <c r="P17" s="27"/>
+      <c r="Q17" s="26">
         <v>23</v>
       </c>
-      <c r="R17" s="24"/>
-      <c r="S17" s="23">
+      <c r="R17" s="27"/>
+      <c r="S17" s="26">
         <v>24</v>
       </c>
-      <c r="T17" s="24"/>
-      <c r="U17" s="23">
+      <c r="T17" s="27"/>
+      <c r="U17" s="26">
         <v>25</v>
       </c>
-      <c r="V17" s="24"/>
-      <c r="W17" s="23">
+      <c r="V17" s="27"/>
+      <c r="W17" s="26">
         <v>26</v>
       </c>
-      <c r="X17" s="24"/>
-      <c r="Y17" s="23">
+      <c r="X17" s="27"/>
+      <c r="Y17" s="26">
         <v>27</v>
       </c>
-      <c r="Z17" s="24"/>
-      <c r="AA17" s="23">
+      <c r="Z17" s="27"/>
+      <c r="AA17" s="26">
         <v>28</v>
       </c>
-      <c r="AB17" s="24"/>
-      <c r="AC17" s="23">
+      <c r="AB17" s="27"/>
+      <c r="AC17" s="26">
         <v>29</v>
       </c>
-      <c r="AD17" s="24"/>
+      <c r="AD17" s="27"/>
+      <c r="AE17" s="26">
+        <v>29</v>
+      </c>
+      <c r="AF17" s="32"/>
     </row>
-    <row r="18" spans="1:30" x14ac:dyDescent="0.35">
-      <c r="A18" s="25" t="s">
+    <row r="18" spans="1:32" x14ac:dyDescent="0.35">
+      <c r="A18" s="23" t="s">
         <v>201</v>
       </c>
       <c r="B18" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="C18" s="15" t="s">
-        <v>395</v>
+      <c r="C18" s="2" t="s">
+        <v>202</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>202</v>
-      </c>
-      <c r="E18" s="2" t="s">
         <v>203</v>
       </c>
+      <c r="E18" s="8" t="s">
+        <v>204</v>
+      </c>
       <c r="F18" s="8" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="G18" s="8" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="H18" s="8" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="I18" s="8" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="J18" s="8" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="K18" s="8" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="L18" s="8" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="M18" s="8" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="N18" s="8" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="O18" s="8" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="P18" s="8" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="Q18" s="8" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="R18" s="8" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="S18" s="8" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="T18" s="8" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="U18" s="8" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="V18" s="8" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="W18" s="8" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="X18" s="8" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="Y18" s="8" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="Z18" s="8" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
       <c r="AA18" s="8" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
       <c r="AB18" s="8" t="s">
-        <v>225</v>
+        <v>402</v>
       </c>
       <c r="AC18" s="8" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="AD18" s="8" t="s">
-        <v>227</v>
+        <v>409</v>
+      </c>
+      <c r="AE18" s="28" t="s">
+        <v>416</v>
+      </c>
+      <c r="AF18" s="8" t="s">
+        <v>423</v>
       </c>
     </row>
-    <row r="19" spans="1:30" x14ac:dyDescent="0.35">
-      <c r="A19" s="26"/>
+    <row r="19" spans="1:32" x14ac:dyDescent="0.35">
+      <c r="A19" s="24"/>
       <c r="B19" s="9"/>
-      <c r="C19" s="20"/>
+      <c r="C19" s="8"/>
       <c r="D19" s="8"/>
       <c r="E19" s="8"/>
       <c r="F19" s="8"/>
@@ -2987,101 +3195,109 @@
       <c r="AB19" s="8"/>
       <c r="AC19" s="8"/>
       <c r="AD19" s="8"/>
+      <c r="AE19" s="28"/>
+      <c r="AF19" s="8"/>
     </row>
-    <row r="20" spans="1:30" x14ac:dyDescent="0.35">
-      <c r="A20" s="26"/>
+    <row r="20" spans="1:32" x14ac:dyDescent="0.35">
+      <c r="A20" s="24"/>
       <c r="B20" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="C20" s="15" t="s">
-        <v>394</v>
+      <c r="C20" s="2" t="s">
+        <v>228</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>228</v>
-      </c>
-      <c r="E20" s="2" t="s">
         <v>229</v>
       </c>
+      <c r="E20" s="8" t="s">
+        <v>230</v>
+      </c>
       <c r="F20" s="8" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="G20" s="8" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="H20" s="8" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="I20" s="8" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="J20" s="8" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="K20" s="8" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="L20" s="8" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="M20" s="8" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="N20" s="8" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="O20" s="8" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="P20" s="8" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="Q20" s="8" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="R20" s="8" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="S20" s="8" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="T20" s="8" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="U20" s="8" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="V20" s="8" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="W20" s="8" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="X20" s="8" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="Y20" s="8" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="Z20" s="8" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="AA20" s="8" t="s">
-        <v>249</v>
+        <v>251</v>
       </c>
       <c r="AB20" s="8" t="s">
-        <v>251</v>
+        <v>401</v>
       </c>
       <c r="AC20" s="8" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="AD20" s="8" t="s">
-        <v>253</v>
+        <v>408</v>
+      </c>
+      <c r="AE20" s="28" t="s">
+        <v>415</v>
+      </c>
+      <c r="AF20" s="8" t="s">
+        <v>422</v>
       </c>
     </row>
-    <row r="21" spans="1:30" x14ac:dyDescent="0.35">
-      <c r="A21" s="26"/>
+    <row r="21" spans="1:32" x14ac:dyDescent="0.35">
+      <c r="A21" s="24"/>
       <c r="B21" s="9"/>
-      <c r="C21" s="20"/>
+      <c r="C21" s="8"/>
       <c r="D21" s="8"/>
       <c r="E21" s="8"/>
       <c r="F21" s="8"/>
@@ -3109,101 +3325,109 @@
       <c r="AB21" s="8"/>
       <c r="AC21" s="8"/>
       <c r="AD21" s="8"/>
+      <c r="AE21" s="28"/>
+      <c r="AF21" s="8"/>
     </row>
-    <row r="22" spans="1:30" x14ac:dyDescent="0.35">
-      <c r="A22" s="26"/>
+    <row r="22" spans="1:32" x14ac:dyDescent="0.35">
+      <c r="A22" s="24"/>
       <c r="B22" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="C22" s="15" t="s">
-        <v>393</v>
+      <c r="C22" s="2" t="s">
+        <v>254</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>254</v>
-      </c>
-      <c r="E22" s="2" t="s">
         <v>255</v>
       </c>
+      <c r="E22" s="8" t="s">
+        <v>256</v>
+      </c>
       <c r="F22" s="8" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="G22" s="8" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="H22" s="8" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="I22" s="8" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="J22" s="8" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="K22" s="8" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="L22" s="8" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="M22" s="8" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="N22" s="8" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="O22" s="8" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="P22" s="8" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="Q22" s="8" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="R22" s="8" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="S22" s="8" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="T22" s="8" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="U22" s="8" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="V22" s="8" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="W22" s="8" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="X22" s="8" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="Y22" s="8" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="Z22" s="8" t="s">
-        <v>276</v>
+        <v>278</v>
       </c>
       <c r="AA22" s="8" t="s">
-        <v>275</v>
+        <v>277</v>
       </c>
       <c r="AB22" s="8" t="s">
-        <v>277</v>
+        <v>400</v>
       </c>
       <c r="AC22" s="8" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="AD22" s="8" t="s">
-        <v>279</v>
+        <v>407</v>
+      </c>
+      <c r="AE22" s="28" t="s">
+        <v>414</v>
+      </c>
+      <c r="AF22" s="8" t="s">
+        <v>421</v>
       </c>
     </row>
-    <row r="23" spans="1:30" x14ac:dyDescent="0.35">
-      <c r="A23" s="26"/>
+    <row r="23" spans="1:32" x14ac:dyDescent="0.35">
+      <c r="A23" s="24"/>
       <c r="B23" s="9"/>
-      <c r="C23" s="20"/>
+      <c r="C23" s="8"/>
       <c r="D23" s="8"/>
       <c r="E23" s="8"/>
       <c r="F23" s="8"/>
@@ -3231,101 +3455,109 @@
       <c r="AB23" s="8"/>
       <c r="AC23" s="8"/>
       <c r="AD23" s="8"/>
+      <c r="AE23" s="28"/>
+      <c r="AF23" s="8"/>
     </row>
-    <row r="24" spans="1:30" x14ac:dyDescent="0.35">
-      <c r="A24" s="26"/>
+    <row r="24" spans="1:32" x14ac:dyDescent="0.35">
+      <c r="A24" s="24"/>
       <c r="B24" s="9" t="s">
         <v>86</v>
       </c>
-      <c r="C24" s="15" t="s">
-        <v>392</v>
+      <c r="C24" s="2" t="s">
+        <v>280</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>280</v>
-      </c>
-      <c r="E24" s="2" t="s">
         <v>281</v>
       </c>
+      <c r="E24" s="8" t="s">
+        <v>282</v>
+      </c>
       <c r="F24" s="8" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="G24" s="8" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="H24" s="8" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="I24" s="8" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="J24" s="8" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="K24" s="8" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="L24" s="8" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="M24" s="8" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="N24" s="8" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="O24" s="8" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="P24" s="8" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="Q24" s="8" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="R24" s="8" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="S24" s="8" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="T24" s="8" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="U24" s="8" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="V24" s="8" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="W24" s="8" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="X24" s="8" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="Y24" s="8" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="Z24" s="8" t="s">
-        <v>302</v>
+        <v>304</v>
       </c>
       <c r="AA24" s="8" t="s">
-        <v>301</v>
+        <v>303</v>
       </c>
       <c r="AB24" s="8" t="s">
-        <v>303</v>
+        <v>399</v>
       </c>
       <c r="AC24" s="8" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="AD24" s="8" t="s">
-        <v>305</v>
+        <v>406</v>
+      </c>
+      <c r="AE24" s="28" t="s">
+        <v>413</v>
+      </c>
+      <c r="AF24" s="8" t="s">
+        <v>420</v>
       </c>
     </row>
-    <row r="25" spans="1:30" x14ac:dyDescent="0.35">
-      <c r="A25" s="26"/>
+    <row r="25" spans="1:32" x14ac:dyDescent="0.35">
+      <c r="A25" s="24"/>
       <c r="B25" s="9"/>
-      <c r="C25" s="20"/>
+      <c r="C25" s="8"/>
       <c r="D25" s="8"/>
       <c r="E25" s="8"/>
       <c r="F25" s="8"/>
@@ -3353,101 +3585,109 @@
       <c r="AB25" s="8"/>
       <c r="AC25" s="8"/>
       <c r="AD25" s="8"/>
+      <c r="AE25" s="28"/>
+      <c r="AF25" s="8"/>
     </row>
-    <row r="26" spans="1:30" x14ac:dyDescent="0.35">
-      <c r="A26" s="26"/>
+    <row r="26" spans="1:32" x14ac:dyDescent="0.35">
+      <c r="A26" s="24"/>
       <c r="B26" s="9" t="s">
         <v>114</v>
       </c>
-      <c r="C26" s="15" t="s">
-        <v>391</v>
+      <c r="C26" s="2" t="s">
+        <v>306</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>306</v>
-      </c>
-      <c r="E26" s="2" t="s">
         <v>307</v>
       </c>
+      <c r="E26" s="8" t="s">
+        <v>308</v>
+      </c>
       <c r="F26" s="8" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="G26" s="8" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="H26" s="8" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="I26" s="8" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="J26" s="8" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="K26" s="8" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="L26" s="8" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="M26" s="8" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="N26" s="8" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="O26" s="8" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="P26" s="8" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="Q26" s="8" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="R26" s="8" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="S26" s="8" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="T26" s="8" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="U26" s="8" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="V26" s="8" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="W26" s="8" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="X26" s="8" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="Y26" s="8" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="Z26" s="8" t="s">
-        <v>328</v>
+        <v>330</v>
       </c>
       <c r="AA26" s="8" t="s">
-        <v>327</v>
+        <v>329</v>
       </c>
       <c r="AB26" s="8" t="s">
-        <v>329</v>
+        <v>398</v>
       </c>
       <c r="AC26" s="8" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="AD26" s="8" t="s">
-        <v>331</v>
+        <v>405</v>
+      </c>
+      <c r="AE26" s="28" t="s">
+        <v>412</v>
+      </c>
+      <c r="AF26" s="8" t="s">
+        <v>419</v>
       </c>
     </row>
-    <row r="27" spans="1:30" x14ac:dyDescent="0.35">
-      <c r="A27" s="26"/>
+    <row r="27" spans="1:32" x14ac:dyDescent="0.35">
+      <c r="A27" s="24"/>
       <c r="B27" s="9"/>
-      <c r="C27" s="20"/>
+      <c r="C27" s="8"/>
       <c r="D27" s="8"/>
       <c r="E27" s="8"/>
       <c r="F27" s="8"/>
@@ -3475,101 +3715,109 @@
       <c r="AB27" s="8"/>
       <c r="AC27" s="8"/>
       <c r="AD27" s="8"/>
+      <c r="AE27" s="28"/>
+      <c r="AF27" s="8"/>
     </row>
-    <row r="28" spans="1:30" x14ac:dyDescent="0.35">
-      <c r="A28" s="26"/>
+    <row r="28" spans="1:32" x14ac:dyDescent="0.35">
+      <c r="A28" s="24"/>
       <c r="B28" s="9" t="s">
         <v>142</v>
       </c>
-      <c r="C28" s="15" t="s">
-        <v>390</v>
+      <c r="C28" s="2" t="s">
+        <v>332</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>332</v>
-      </c>
-      <c r="E28" s="2" t="s">
         <v>333</v>
       </c>
+      <c r="E28" s="8" t="s">
+        <v>334</v>
+      </c>
       <c r="F28" s="8" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="G28" s="8" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="H28" s="8" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="I28" s="8" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="J28" s="8" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="K28" s="8" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="L28" s="8" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="M28" s="8" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="N28" s="8" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="O28" s="8" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="P28" s="8" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="Q28" s="8" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="R28" s="8" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="S28" s="8" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="T28" s="8" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="U28" s="8" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="V28" s="8" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="W28" s="8" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="X28" s="8" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="Y28" s="8" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="Z28" s="8" t="s">
-        <v>354</v>
+        <v>356</v>
       </c>
       <c r="AA28" s="8" t="s">
-        <v>353</v>
+        <v>355</v>
       </c>
       <c r="AB28" s="8" t="s">
-        <v>355</v>
+        <v>397</v>
       </c>
       <c r="AC28" s="8" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="AD28" s="8" t="s">
-        <v>357</v>
+        <v>404</v>
+      </c>
+      <c r="AE28" s="28" t="s">
+        <v>411</v>
+      </c>
+      <c r="AF28" s="8" t="s">
+        <v>418</v>
       </c>
     </row>
-    <row r="29" spans="1:30" x14ac:dyDescent="0.35">
-      <c r="A29" s="26"/>
+    <row r="29" spans="1:32" x14ac:dyDescent="0.35">
+      <c r="A29" s="24"/>
       <c r="B29" s="9"/>
-      <c r="C29" s="20"/>
+      <c r="C29" s="16"/>
       <c r="D29" s="16"/>
       <c r="E29" s="16"/>
       <c r="F29" s="16"/>
@@ -3597,99 +3845,107 @@
       <c r="AB29" s="16"/>
       <c r="AC29" s="16"/>
       <c r="AD29" s="16"/>
+      <c r="AE29" s="29"/>
+      <c r="AF29" s="16"/>
     </row>
-    <row r="30" spans="1:30" x14ac:dyDescent="0.35">
-      <c r="A30" s="26"/>
+    <row r="30" spans="1:32" x14ac:dyDescent="0.35">
+      <c r="A30" s="24"/>
       <c r="B30" s="9" t="s">
         <v>170</v>
       </c>
       <c r="C30" s="15" t="s">
-        <v>199</v>
+        <v>358</v>
       </c>
       <c r="D30" s="15" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="E30" s="15" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="F30" s="15" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="G30" s="15" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="H30" s="15" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="I30" s="15" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="J30" s="15" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="K30" s="15" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="L30" s="15" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="M30" s="15" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="N30" s="15" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="O30" s="15" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="P30" s="15" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="Q30" s="15" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="R30" s="15" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="S30" s="15" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="T30" s="15" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="U30" s="15" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="V30" s="15" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="W30" s="15" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="X30" s="15" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="Y30" s="15" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="Z30" s="15" t="s">
-        <v>380</v>
+        <v>382</v>
       </c>
       <c r="AA30" s="15" t="s">
-        <v>379</v>
+        <v>381</v>
       </c>
       <c r="AB30" s="15" t="s">
-        <v>381</v>
+        <v>396</v>
       </c>
       <c r="AC30" s="15" t="s">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="AD30" s="15" t="s">
-        <v>383</v>
+        <v>403</v>
+      </c>
+      <c r="AE30" s="30" t="s">
+        <v>410</v>
+      </c>
+      <c r="AF30" s="15" t="s">
+        <v>417</v>
       </c>
     </row>
-    <row r="31" spans="1:30" ht="21.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="27"/>
+    <row r="31" spans="1:32" ht="21.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A31" s="25"/>
       <c r="B31" s="9"/>
       <c r="C31" s="17"/>
       <c r="D31" s="17"/>
@@ -3698,7 +3954,7 @@
       <c r="G31" s="17"/>
       <c r="H31" s="17"/>
       <c r="I31" s="17"/>
-      <c r="J31" s="17"/>
+      <c r="J31" s="18"/>
       <c r="K31" s="18"/>
       <c r="L31" s="18"/>
       <c r="M31" s="18"/>
@@ -3719,8 +3975,10 @@
       <c r="AB31" s="18"/>
       <c r="AC31" s="18"/>
       <c r="AD31" s="18"/>
+      <c r="AE31" s="31"/>
+      <c r="AF31" s="33"/>
     </row>
-    <row r="32" spans="1:30" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:32" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A32" s="10"/>
       <c r="B32" s="10"/>
       <c r="C32" s="11"/>
@@ -3751,26 +4009,13 @@
       <c r="AB32" s="12"/>
       <c r="AC32" s="12"/>
       <c r="AD32" s="12"/>
+      <c r="AE32" s="12"/>
+      <c r="AF32" s="12"/>
     </row>
   </sheetData>
-  <mergeCells count="30">
-    <mergeCell ref="A2:A15"/>
-    <mergeCell ref="A18:A31"/>
-    <mergeCell ref="AA17:AB17"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="I17:J17"/>
-    <mergeCell ref="I1:J1"/>
-    <mergeCell ref="K17:L17"/>
-    <mergeCell ref="M17:N17"/>
-    <mergeCell ref="G1:H1"/>
-    <mergeCell ref="C1:D1"/>
-    <mergeCell ref="E1:F1"/>
-    <mergeCell ref="K1:L1"/>
-    <mergeCell ref="W1:X1"/>
-    <mergeCell ref="O1:P1"/>
-    <mergeCell ref="Q1:R1"/>
-    <mergeCell ref="S1:T1"/>
-    <mergeCell ref="U1:V1"/>
+  <mergeCells count="32">
+    <mergeCell ref="AE1:AF1"/>
+    <mergeCell ref="AE17:AF17"/>
     <mergeCell ref="AC17:AD17"/>
     <mergeCell ref="AA1:AB1"/>
     <mergeCell ref="M1:N1"/>
@@ -3784,6 +4029,23 @@
     <mergeCell ref="O17:P17"/>
     <mergeCell ref="Q17:R17"/>
     <mergeCell ref="W17:X17"/>
+    <mergeCell ref="W1:X1"/>
+    <mergeCell ref="O1:P1"/>
+    <mergeCell ref="Q1:R1"/>
+    <mergeCell ref="S1:T1"/>
+    <mergeCell ref="U1:V1"/>
+    <mergeCell ref="I1:J1"/>
+    <mergeCell ref="K17:L17"/>
+    <mergeCell ref="M17:N17"/>
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="K1:L1"/>
+    <mergeCell ref="A2:A15"/>
+    <mergeCell ref="A18:A31"/>
+    <mergeCell ref="AA17:AB17"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="I17:J17"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" fitToHeight="0" orientation="landscape"/>

</xml_diff>